<commit_message>
UpdateVersion: Bugfix for key_row
</commit_message>
<xml_diff>
--- a/test/test_old.xlsx
+++ b/test/test_old.xlsx
@@ -1297,17 +1297,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffff00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1327,10 +1322,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -2220,53 +2214,53 @@
       <c r="AC10" t="s"/>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="1" t="s"/>
-      <c r="C11" s="1" t="n">
+      <c r="B11" t="s"/>
+      <c r="C11" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="1" t="s"/>
-      <c r="E11" s="1" t="s">
+      <c r="D11" t="s"/>
+      <c r="E11" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="1" t="s"/>
-      <c r="K11" s="1" t="s"/>
-      <c r="L11" s="1" t="s">
+      <c r="J11" t="s"/>
+      <c r="K11" t="s"/>
+      <c r="L11" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="1" t="s"/>
-      <c r="O11" s="1" t="s"/>
-      <c r="P11" s="1" t="s"/>
-      <c r="Q11" s="1" t="s"/>
-      <c r="R11" s="1" t="s"/>
-      <c r="S11" s="1" t="s"/>
-      <c r="T11" s="1" t="s"/>
-      <c r="U11" s="1" t="s"/>
-      <c r="V11" s="1" t="s"/>
-      <c r="W11" s="1" t="s"/>
-      <c r="X11" s="1" t="s"/>
-      <c r="Y11" s="1" t="s"/>
-      <c r="Z11" s="1" t="s"/>
-      <c r="AA11" s="1" t="s"/>
-      <c r="AB11" s="1" t="s"/>
-      <c r="AC11" s="1" t="s"/>
+      <c r="N11" t="s"/>
+      <c r="O11" t="s"/>
+      <c r="P11" t="s"/>
+      <c r="Q11" t="s"/>
+      <c r="R11" t="s"/>
+      <c r="S11" t="s"/>
+      <c r="T11" t="s"/>
+      <c r="U11" t="s"/>
+      <c r="V11" t="s"/>
+      <c r="W11" t="s"/>
+      <c r="X11" t="s"/>
+      <c r="Y11" t="s"/>
+      <c r="Z11" t="s"/>
+      <c r="AA11" t="s"/>
+      <c r="AB11" t="s"/>
+      <c r="AC11" t="s"/>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" t="s">
@@ -2314,53 +2308,53 @@
       <c r="AC12" t="s"/>
     </row>
     <row r="13" spans="1:29">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="2" t="s"/>
-      <c r="C13" s="2" t="n">
+      <c r="B13" s="1" t="s"/>
+      <c r="C13" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="D13" s="2" t="s"/>
-      <c r="E13" s="2" t="s"/>
-      <c r="F13" s="2" t="s">
+      <c r="D13" s="1" t="s"/>
+      <c r="E13" s="1" t="s"/>
+      <c r="F13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="2" t="s"/>
-      <c r="J13" s="2" t="s"/>
-      <c r="K13" s="2" t="s"/>
-      <c r="L13" s="2" t="s">
+      <c r="I13" s="1" t="s"/>
+      <c r="J13" s="1" t="s"/>
+      <c r="K13" s="1" t="s"/>
+      <c r="L13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="M13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="N13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P13" s="2" t="s"/>
-      <c r="Q13" s="2" t="s"/>
-      <c r="R13" s="2" t="s"/>
-      <c r="S13" s="2" t="s"/>
-      <c r="T13" s="2" t="s"/>
-      <c r="U13" s="2" t="s"/>
-      <c r="V13" s="2" t="s"/>
-      <c r="W13" s="2" t="s"/>
-      <c r="X13" s="2" t="s"/>
-      <c r="Y13" s="2" t="s"/>
-      <c r="Z13" s="2" t="s"/>
-      <c r="AA13" s="2" t="s"/>
-      <c r="AB13" s="2" t="s"/>
-      <c r="AC13" s="2" t="s"/>
+      <c r="P13" s="1" t="s"/>
+      <c r="Q13" s="1" t="s"/>
+      <c r="R13" s="1" t="s"/>
+      <c r="S13" s="1" t="s"/>
+      <c r="T13" s="1" t="s"/>
+      <c r="U13" s="1" t="s"/>
+      <c r="V13" s="1" t="s"/>
+      <c r="W13" s="1" t="s"/>
+      <c r="X13" s="1" t="s"/>
+      <c r="Y13" s="1" t="s"/>
+      <c r="Z13" s="1" t="s"/>
+      <c r="AA13" s="1" t="s"/>
+      <c r="AB13" s="1" t="s"/>
+      <c r="AC13" s="1" t="s"/>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" t="s">
@@ -2408,53 +2402,53 @@
       <c r="AC14" t="s"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="2" t="s"/>
-      <c r="C15" s="2" t="n">
+      <c r="B15" s="1" t="s"/>
+      <c r="C15" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="D15" s="2" t="s"/>
-      <c r="E15" s="2" t="s"/>
-      <c r="F15" s="2" t="s">
+      <c r="D15" s="1" t="s"/>
+      <c r="E15" s="1" t="s"/>
+      <c r="F15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="2" t="s"/>
-      <c r="J15" s="2" t="s"/>
-      <c r="K15" s="2" t="s"/>
-      <c r="L15" s="2" t="s">
+      <c r="I15" s="1" t="s"/>
+      <c r="J15" s="1" t="s"/>
+      <c r="K15" s="1" t="s"/>
+      <c r="L15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P15" s="2" t="s"/>
-      <c r="Q15" s="2" t="s"/>
-      <c r="R15" s="2" t="s"/>
-      <c r="S15" s="2" t="s"/>
-      <c r="T15" s="2" t="s"/>
-      <c r="U15" s="2" t="s"/>
-      <c r="V15" s="2" t="s"/>
-      <c r="W15" s="2" t="s"/>
-      <c r="X15" s="2" t="s"/>
-      <c r="Y15" s="2" t="s"/>
-      <c r="Z15" s="2" t="s"/>
-      <c r="AA15" s="2" t="s"/>
-      <c r="AB15" s="2" t="s"/>
-      <c r="AC15" s="2" t="s"/>
+      <c r="P15" s="1" t="s"/>
+      <c r="Q15" s="1" t="s"/>
+      <c r="R15" s="1" t="s"/>
+      <c r="S15" s="1" t="s"/>
+      <c r="T15" s="1" t="s"/>
+      <c r="U15" s="1" t="s"/>
+      <c r="V15" s="1" t="s"/>
+      <c r="W15" s="1" t="s"/>
+      <c r="X15" s="1" t="s"/>
+      <c r="Y15" s="1" t="s"/>
+      <c r="Z15" s="1" t="s"/>
+      <c r="AA15" s="1" t="s"/>
+      <c r="AB15" s="1" t="s"/>
+      <c r="AC15" s="1" t="s"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" t="s">

</xml_diff>